<commit_message>
adding in missed reference sequences
</commit_message>
<xml_diff>
--- a/PySimPlot/pysimplot_references.xlsx
+++ b/PySimPlot/pysimplot_references.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gwenddolenkettenburg/Desktop/developer/mada-bat-picornavirus/PySimPlot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23748F4B-55D6-D542-8D55-924804C4C0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B79487D-4923-B94E-A60A-C7D12FC01890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-1980" windowWidth="16100" windowHeight="18820" xr2:uid="{D098B555-783A-FB4C-A4D2-95855C80ECD2}"/>
+    <workbookView xWindow="180" yWindow="740" windowWidth="22840" windowHeight="17360" xr2:uid="{D098B555-783A-FB4C-A4D2-95855C80ECD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="334">
   <si>
     <t>cardiovirus</t>
   </si>
@@ -347,15 +347,9 @@
     <t>YP_009345901.1</t>
   </si>
   <si>
-    <t>WXG28554.1</t>
-  </si>
-  <si>
     <t>Bat sapovirus</t>
   </si>
   <si>
-    <t>Bat sapovirus BtSY2</t>
-  </si>
-  <si>
     <t>Bat sapovirus WD3</t>
   </si>
   <si>
@@ -365,45 +359,12 @@
     <t>WBG95506.1</t>
   </si>
   <si>
-    <t>WBV74378.1</t>
-  </si>
-  <si>
-    <t>WGC86364.1</t>
-  </si>
-  <si>
     <t>Pteropodidae bat teschovirus</t>
   </si>
   <si>
-    <t>WXG28556.1</t>
-  </si>
-  <si>
-    <t>WXG28549.1</t>
-  </si>
-  <si>
     <t>Bat picornavirus BtSY4</t>
   </si>
   <si>
-    <t>Bat picornavirus 3</t>
-  </si>
-  <si>
-    <t>Wilde virus-3</t>
-  </si>
-  <si>
-    <t>WBV74372.1</t>
-  </si>
-  <si>
-    <t>QQR34440.1</t>
-  </si>
-  <si>
-    <t>WFG77366.1</t>
-  </si>
-  <si>
-    <t>AEM23662.1</t>
-  </si>
-  <si>
-    <t>WFG77375.1</t>
-  </si>
-  <si>
     <t>blastx_host</t>
   </si>
   <si>
@@ -428,63 +389,21 @@
     <t>Eonycteris spelaea - China</t>
   </si>
   <si>
-    <t>Rhinolophus marshalli - China</t>
-  </si>
-  <si>
-    <t>Vulpes vulpes - Australia</t>
-  </si>
-  <si>
     <t>Rhinolophus sinicus - China</t>
   </si>
   <si>
-    <t>Hipposideros armiger - China</t>
-  </si>
-  <si>
-    <t>Rhinolophus pusillus - China</t>
-  </si>
-  <si>
     <t>Rousettus bat picornavirus</t>
   </si>
   <si>
     <t>Chaerephon bat picornavirus</t>
   </si>
   <si>
-    <t>Shanbavirus A</t>
-  </si>
-  <si>
-    <t>teschovirus A6</t>
-  </si>
-  <si>
-    <t>KJ641693.1</t>
-  </si>
-  <si>
-    <t>Shanbavirus</t>
-  </si>
-  <si>
-    <t>OQ363777.1</t>
-  </si>
-  <si>
-    <t>OR951335.1</t>
-  </si>
-  <si>
-    <t>Teschovirus sp.</t>
-  </si>
-  <si>
-    <t>KX420938.1</t>
-  </si>
-  <si>
     <t>OR951334.1</t>
   </si>
   <si>
     <t>Rousettus bat calicivirus</t>
   </si>
   <si>
-    <t>OR951145.1</t>
-  </si>
-  <si>
-    <t>OP963623.1</t>
-  </si>
-  <si>
     <t>Eidolon bat picornavirus</t>
   </si>
   <si>
@@ -623,9 +542,6 @@
     <t>Rousettus aegyptiacus - Kenya</t>
   </si>
   <si>
-    <t>Eonycteris spelaea -China</t>
-  </si>
-  <si>
     <t>KX759623.1</t>
   </si>
   <si>
@@ -641,9 +557,6 @@
     <t>PP712004.1</t>
   </si>
   <si>
-    <t>OP930876.1</t>
-  </si>
-  <si>
     <t>OQ709197.1</t>
   </si>
   <si>
@@ -659,15 +572,6 @@
     <t>OR951333.1</t>
   </si>
   <si>
-    <t>MT295502.1</t>
-  </si>
-  <si>
-    <t>Tibetan pig - China</t>
-  </si>
-  <si>
-    <t>Eidolon helvum - Saudi Arabia</t>
-  </si>
-  <si>
     <t>PP711945.1</t>
   </si>
   <si>
@@ -680,33 +584,12 @@
     <t>PP711946.1</t>
   </si>
   <si>
-    <t>NC_015934.1</t>
-  </si>
-  <si>
-    <t>OP963670.1</t>
-  </si>
-  <si>
-    <t>OQ363764.1</t>
-  </si>
-  <si>
-    <t>HQ595345.1</t>
-  </si>
-  <si>
-    <t>OQ363775.1</t>
-  </si>
-  <si>
-    <t>Rhinolophus hipposideros - China</t>
-  </si>
-  <si>
     <t>OP834152.1</t>
   </si>
   <si>
     <t>OQ716001.1</t>
   </si>
   <si>
-    <t>OP963617.1</t>
-  </si>
-  <si>
     <t>number</t>
   </si>
   <si>
@@ -719,24 +602,9 @@
     <t>close ref</t>
   </si>
   <si>
-    <t>HQ595340.1</t>
-  </si>
-  <si>
-    <t>HQ595342.1</t>
-  </si>
-  <si>
-    <t>HQ595344.1</t>
-  </si>
-  <si>
     <t>refseq</t>
   </si>
   <si>
-    <t>Bat picornavirus 1</t>
-  </si>
-  <si>
-    <t>Bat picornavirus 2</t>
-  </si>
-  <si>
     <t>MG875515</t>
   </si>
   <si>
@@ -1016,9 +884,6 @@
     <t>Swine - Japan</t>
   </si>
   <si>
-    <t>Miniopterus magnater - China</t>
-  </si>
-  <si>
     <t>cardio_align_nt</t>
   </si>
   <si>
@@ -1070,41 +935,116 @@
     <t>sapelo_align_aa</t>
   </si>
   <si>
-    <t>1,2,3,12,13,15,16</t>
-  </si>
-  <si>
     <t>sapo_align_nt</t>
   </si>
   <si>
     <t>sapo_align_aa</t>
   </si>
   <si>
-    <t>1,6,15,16,17,19</t>
-  </si>
-  <si>
     <t>tescho_align_nt</t>
   </si>
   <si>
     <t>tescho_align_aa</t>
   </si>
   <si>
-    <t>1,2,3,4,5,6</t>
-  </si>
-  <si>
     <t>batpicorna_align_nt</t>
   </si>
   <si>
     <t>batpicorna_align_aa</t>
   </si>
   <si>
-    <t>1,2,4,8,9,10,12</t>
+    <t>XBH23993.1</t>
+  </si>
+  <si>
+    <t>XBH23983.1</t>
+  </si>
+  <si>
+    <t>XBH24168.1</t>
+  </si>
+  <si>
+    <t>XBH24156.1</t>
+  </si>
+  <si>
+    <t>XBH24177.1</t>
+  </si>
+  <si>
+    <t>XBH24178.1</t>
+  </si>
+  <si>
+    <t>PP712008.1</t>
+  </si>
+  <si>
+    <t>PP712015.1</t>
+  </si>
+  <si>
+    <t>XBH24020.1</t>
+  </si>
+  <si>
+    <t>XBH24006.1</t>
+  </si>
+  <si>
+    <t>PP711948.1</t>
+  </si>
+  <si>
+    <t>XBH24017.1</t>
+  </si>
+  <si>
+    <t>XBH23984.1</t>
+  </si>
+  <si>
+    <t>Rousettus aegypticus - Uganda</t>
+  </si>
+  <si>
+    <t>PP711912.1</t>
+  </si>
+  <si>
+    <t>KX759619.1</t>
+  </si>
+  <si>
+    <t>OP963622.1</t>
+  </si>
+  <si>
+    <t>Bat sapovirus BtSY1</t>
+  </si>
+  <si>
+    <t>Cynopterus sphinx - China</t>
+  </si>
+  <si>
+    <t>OR951325.1</t>
+  </si>
+  <si>
+    <t>Rousettus aegypticus - Kenya</t>
+  </si>
+  <si>
+    <t>PP711913.1</t>
+  </si>
+  <si>
+    <t>PP711930.1</t>
+  </si>
+  <si>
+    <t>PP711928.1</t>
+  </si>
+  <si>
+    <t>Bat picornavirus 7</t>
+  </si>
+  <si>
+    <t>PP745912.1</t>
+  </si>
+  <si>
+    <t>Taphozous melanopogon - China</t>
+  </si>
+  <si>
+    <t>PP711909.1</t>
+  </si>
+  <si>
+    <t>PP746000.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1121,6 +1061,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -1163,13 +1109,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D3F017-F6A7-2E48-AA72-A9E646068FC2}">
-  <dimension ref="A2:H215"/>
+  <dimension ref="A2:I211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="D215" sqref="D215"/>
+    <sheetView tabSelected="1" topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="C156" sqref="C156:C158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1524,7 +1476,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1545,14 +1497,14 @@
         <v>88</v>
       </c>
       <c r="H3" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -1571,47 +1523,47 @@
         <v>90</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>166</v>
+      <c r="B5" s="4" t="s">
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>89</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E5" s="2">
         <v>7629</v>
       </c>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>164</v>
+      <c r="B6" s="4" t="s">
+        <v>137</v>
       </c>
       <c r="C6" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E6" s="2">
         <v>7548</v>
       </c>
       <c r="H6" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1619,19 +1571,19 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
       <c r="C7" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="D7" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E7" s="2">
         <v>7724</v>
       </c>
       <c r="H7" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -1639,19 +1591,19 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
       <c r="C8" t="s">
-        <v>286</v>
+        <v>242</v>
       </c>
       <c r="D8" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E8" s="2">
         <v>7890</v>
       </c>
       <c r="H8" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1659,19 +1611,19 @@
         <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
       <c r="C9" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
       <c r="D9" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E9" s="2">
         <v>8530</v>
       </c>
       <c r="H9" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -1679,19 +1631,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
       <c r="C10" t="s">
-        <v>292</v>
+        <v>248</v>
       </c>
       <c r="D10" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E10" s="2">
         <v>8122</v>
       </c>
       <c r="H10" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -1699,19 +1651,19 @@
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
       <c r="C11" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
       <c r="D11" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E11" s="2">
         <v>7835</v>
       </c>
       <c r="H11" t="s">
-        <v>295</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -1719,19 +1671,19 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>297</v>
+        <v>253</v>
       </c>
       <c r="C12" t="s">
-        <v>296</v>
+        <v>252</v>
       </c>
       <c r="D12" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E12" s="2">
         <v>8115</v>
       </c>
       <c r="H12" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1739,43 +1691,43 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C13" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
       <c r="D13" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E13" s="2">
         <v>8101</v>
       </c>
       <c r="H13" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B15" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>327</v>
+        <v>282</v>
       </c>
       <c r="B16" t="s">
-        <v>329</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>328</v>
+        <v>283</v>
       </c>
       <c r="B17" t="s">
-        <v>329</v>
+        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1785,7 +1737,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
@@ -1806,7 +1758,7 @@
         <v>88</v>
       </c>
       <c r="H22" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1832,14 +1784,14 @@
         <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C24" t="s">
@@ -1858,14 +1810,14 @@
         <v>92</v>
       </c>
       <c r="H24" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C25" t="s">
@@ -1884,7 +1836,7 @@
         <v>92</v>
       </c>
       <c r="H25" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1910,47 +1862,47 @@
         <v>92</v>
       </c>
       <c r="H26" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>5</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>160</v>
+      <c r="B27" s="4" t="s">
+        <v>133</v>
       </c>
       <c r="C27" t="s">
         <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E27" s="2">
         <v>7333</v>
       </c>
       <c r="H27" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>6</v>
       </c>
-      <c r="B28" s="5" t="s">
-        <v>169</v>
+      <c r="B28" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="C28" t="s">
-        <v>161</v>
+        <v>134</v>
       </c>
       <c r="D28" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E28" s="2">
         <v>7417</v>
       </c>
       <c r="H28" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1958,19 +1910,19 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="D29" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E29" s="2">
         <v>6839</v>
       </c>
       <c r="H29" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1978,19 +1930,19 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
       <c r="C30" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
       <c r="D30" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E30" s="2">
         <v>7478</v>
       </c>
       <c r="H30" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1998,39 +1950,39 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
       <c r="C31" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="D31" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E31" s="2">
         <v>7476</v>
       </c>
       <c r="H31" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>10</v>
       </c>
-      <c r="B32" s="5" t="s">
-        <v>279</v>
+      <c r="B32" s="4" t="s">
+        <v>235</v>
       </c>
       <c r="C32" t="s">
-        <v>271</v>
+        <v>227</v>
       </c>
       <c r="D32" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E32" s="2">
         <v>7570</v>
       </c>
       <c r="H32" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -2038,19 +1990,19 @@
         <v>11</v>
       </c>
       <c r="B33" t="s">
-        <v>280</v>
+        <v>236</v>
       </c>
       <c r="C33" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
       <c r="D33" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E33" s="2">
         <v>7656</v>
       </c>
       <c r="H33" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -2058,19 +2010,19 @@
         <v>12</v>
       </c>
       <c r="B34" t="s">
-        <v>281</v>
+        <v>237</v>
       </c>
       <c r="C34" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
       <c r="D34" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E34" s="2">
         <v>7406</v>
       </c>
       <c r="H34" t="s">
-        <v>305</v>
+        <v>261</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -2078,19 +2030,19 @@
         <v>13</v>
       </c>
       <c r="B35" t="s">
-        <v>282</v>
+        <v>238</v>
       </c>
       <c r="C35" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="D35" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E35" s="2">
         <v>7563</v>
       </c>
       <c r="H35" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -2098,19 +2050,19 @@
         <v>14</v>
       </c>
       <c r="B36" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="C36" t="s">
-        <v>275</v>
+        <v>231</v>
       </c>
       <c r="D36" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E36" s="2">
         <v>7399</v>
       </c>
-      <c r="H36" s="4" t="s">
-        <v>307</v>
+      <c r="H36" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -2118,43 +2070,43 @@
         <v>15</v>
       </c>
       <c r="B37" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="C37" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
       <c r="D37" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E37" s="2">
         <v>7810</v>
       </c>
-      <c r="H37" s="4" t="s">
-        <v>308</v>
+      <c r="H37" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B39" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>330</v>
+        <v>285</v>
       </c>
       <c r="B40" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>331</v>
+        <v>286</v>
       </c>
       <c r="B41" t="s">
-        <v>332</v>
+        <v>287</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2164,7 +2116,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B46" t="s">
         <v>1</v>
@@ -2185,14 +2137,14 @@
         <v>88</v>
       </c>
       <c r="H46" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C47" t="s">
@@ -2211,7 +2163,7 @@
         <v>94</v>
       </c>
       <c r="H47" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2237,7 +2189,7 @@
         <v>95</v>
       </c>
       <c r="H48" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -2263,7 +2215,7 @@
         <v>94</v>
       </c>
       <c r="H49" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2289,7 +2241,7 @@
         <v>94</v>
       </c>
       <c r="H50" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2315,7 +2267,7 @@
         <v>94</v>
       </c>
       <c r="H51" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2341,7 +2293,7 @@
         <v>95</v>
       </c>
       <c r="H52" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2367,14 +2319,14 @@
         <v>94</v>
       </c>
       <c r="H53" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>8</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C54" t="s">
@@ -2393,27 +2345,27 @@
         <v>94</v>
       </c>
       <c r="H54" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>9</v>
       </c>
-      <c r="B55" s="5" t="s">
-        <v>174</v>
+      <c r="B55" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="C55" t="s">
         <v>16</v>
       </c>
       <c r="D55" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E55" s="2">
         <v>8263</v>
       </c>
       <c r="H55" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2421,19 +2373,19 @@
         <v>10</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="C56" t="s">
         <v>93</v>
       </c>
       <c r="D56" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E56">
         <v>1120</v>
       </c>
       <c r="H56" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2441,19 +2393,19 @@
         <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="C57" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="D57" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E57">
         <v>3027</v>
       </c>
       <c r="H57" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2461,19 +2413,19 @@
         <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="C58" t="s">
-        <v>159</v>
+        <v>132</v>
       </c>
       <c r="D58" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E58">
         <v>1508</v>
       </c>
       <c r="H58" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2481,19 +2433,19 @@
         <v>13</v>
       </c>
       <c r="B59" t="s">
-        <v>263</v>
+        <v>219</v>
       </c>
       <c r="C59" t="s">
-        <v>257</v>
+        <v>213</v>
       </c>
       <c r="D59" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E59" s="1">
         <v>8280</v>
       </c>
       <c r="H59" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2501,19 +2453,19 @@
         <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
       <c r="C60" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
       <c r="D60" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E60" s="1">
         <v>8374</v>
       </c>
       <c r="H60" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2521,19 +2473,19 @@
         <v>15</v>
       </c>
       <c r="B61" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
       <c r="C61" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
       <c r="D61" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E61" s="1">
         <v>8210</v>
       </c>
       <c r="H61" t="s">
-        <v>312</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2541,19 +2493,19 @@
         <v>16</v>
       </c>
       <c r="B62" t="s">
-        <v>266</v>
+        <v>222</v>
       </c>
       <c r="C62" t="s">
-        <v>260</v>
+        <v>216</v>
       </c>
       <c r="D62" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E62" s="1">
         <v>8087</v>
       </c>
       <c r="H62" t="s">
-        <v>313</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2561,19 +2513,19 @@
         <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
       <c r="C63" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="D63" t="s">
-        <v>230</v>
-      </c>
-      <c r="E63" s="3">
+        <v>188</v>
+      </c>
+      <c r="E63">
         <v>2086</v>
       </c>
       <c r="H63" t="s">
-        <v>314</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2581,43 +2533,43 @@
         <v>18</v>
       </c>
       <c r="B64" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
       <c r="C64" t="s">
-        <v>262</v>
+        <v>218</v>
       </c>
       <c r="D64" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E64" s="1">
         <v>7555</v>
       </c>
       <c r="H64" t="s">
-        <v>315</v>
+        <v>271</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B66" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>334</v>
+        <v>289</v>
       </c>
       <c r="B67" t="s">
-        <v>335</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>333</v>
+        <v>288</v>
       </c>
       <c r="B68" t="s">
-        <v>335</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2627,7 +2579,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B73" t="s">
         <v>1</v>
@@ -2648,14 +2600,14 @@
         <v>88</v>
       </c>
       <c r="H73" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C74" t="s">
@@ -2674,47 +2626,47 @@
         <v>97</v>
       </c>
       <c r="H74" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2</v>
       </c>
-      <c r="B75" s="5" t="s">
-        <v>179</v>
+      <c r="B75" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="C75" t="s">
         <v>96</v>
       </c>
       <c r="D75" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E75" s="2">
         <v>7092</v>
       </c>
       <c r="H75" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>3</v>
       </c>
-      <c r="B76" s="5" t="s">
-        <v>180</v>
+      <c r="B76" s="4" t="s">
+        <v>153</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="D76" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E76" s="2">
         <v>7482</v>
       </c>
       <c r="H76" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
@@ -2722,19 +2674,19 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>254</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>252</v>
+        <v>208</v>
       </c>
       <c r="D77" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E77" s="2">
         <v>7272</v>
       </c>
       <c r="H77" t="s">
-        <v>316</v>
+        <v>272</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2742,13 +2694,13 @@
         <v>5</v>
       </c>
       <c r="B78" t="s">
-        <v>255</v>
+        <v>211</v>
       </c>
       <c r="C78" t="s">
         <v>96</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E78" s="2">
         <v>7092</v>
@@ -2759,13 +2711,13 @@
         <v>6</v>
       </c>
       <c r="B79" t="s">
-        <v>256</v>
+        <v>212</v>
       </c>
       <c r="C79" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
       <c r="D79" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E79" s="2">
         <v>7429</v>
@@ -2773,26 +2725,26 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B81" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>336</v>
+        <v>291</v>
       </c>
       <c r="B82" t="s">
-        <v>338</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>337</v>
+        <v>292</v>
       </c>
       <c r="B83" t="s">
-        <v>338</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2802,7 +2754,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B88" t="s">
         <v>1</v>
@@ -2823,14 +2775,14 @@
         <v>88</v>
       </c>
       <c r="H88" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C89" t="s">
@@ -2849,47 +2801,47 @@
         <v>99</v>
       </c>
       <c r="H89" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>2</v>
       </c>
-      <c r="B90" s="5" t="s">
-        <v>182</v>
+      <c r="B90" s="4" t="s">
+        <v>155</v>
       </c>
       <c r="C90" t="s">
         <v>98</v>
       </c>
       <c r="D90" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E90" s="2">
         <v>8096</v>
       </c>
       <c r="H90" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>3</v>
       </c>
-      <c r="B91" s="5" t="s">
-        <v>152</v>
+      <c r="B91" s="4" t="s">
+        <v>125</v>
       </c>
       <c r="C91" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="D91" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E91" s="2">
         <v>6961</v>
       </c>
       <c r="H91" t="s">
-        <v>183</v>
+        <v>156</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2897,19 +2849,19 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>154</v>
+        <v>127</v>
       </c>
       <c r="C92" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="D92" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E92">
         <v>3238</v>
       </c>
       <c r="H92" t="s">
-        <v>184</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2917,19 +2869,19 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>185</v>
+        <v>158</v>
       </c>
       <c r="C93" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="D93" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E93" s="2">
         <v>8029</v>
       </c>
       <c r="H93" t="s">
-        <v>186</v>
+        <v>159</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2937,39 +2889,39 @@
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="C94" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="D94" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E94" s="2">
         <v>7161</v>
       </c>
       <c r="H94" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>7</v>
       </c>
-      <c r="B95" s="5" t="s">
-        <v>243</v>
+      <c r="B95" s="4" t="s">
+        <v>199</v>
       </c>
       <c r="C95" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
       <c r="D95" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E95" s="2">
         <v>8468</v>
       </c>
       <c r="H95" t="s">
-        <v>317</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -2977,19 +2929,19 @@
         <v>8</v>
       </c>
       <c r="B96" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="C96" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="D96" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E96" s="2">
         <v>6855</v>
       </c>
       <c r="H96" t="s">
-        <v>318</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -2997,19 +2949,19 @@
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
       <c r="C97" t="s">
-        <v>249</v>
+        <v>205</v>
       </c>
       <c r="D97" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E97" s="2">
         <v>8096</v>
       </c>
       <c r="H97" t="s">
-        <v>319</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -3017,19 +2969,19 @@
         <v>10</v>
       </c>
       <c r="B98" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
       <c r="C98" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
       <c r="D98" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E98" s="2">
         <v>7618</v>
       </c>
       <c r="H98" t="s">
-        <v>320</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -3037,43 +2989,43 @@
         <v>11</v>
       </c>
       <c r="B99" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
       <c r="C99" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
       <c r="D99" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E99" s="2">
         <v>7407</v>
       </c>
       <c r="H99" t="s">
-        <v>321</v>
+        <v>277</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B101" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>340</v>
+        <v>295</v>
       </c>
       <c r="B102" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>339</v>
+        <v>294</v>
       </c>
       <c r="B103" t="s">
-        <v>341</v>
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3083,7 +3035,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B109" t="s">
         <v>1</v>
@@ -3104,14 +3056,14 @@
         <v>88</v>
       </c>
       <c r="H109" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>1</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C110" t="s">
@@ -3130,14 +3082,14 @@
         <v>102</v>
       </c>
       <c r="H110" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C111" t="s">
@@ -3150,20 +3102,20 @@
         <v>7751</v>
       </c>
       <c r="F111" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="G111" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="H111" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>3</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="4" t="s">
         <v>36</v>
       </c>
       <c r="C112" t="s">
@@ -3176,13 +3128,13 @@
         <v>7714</v>
       </c>
       <c r="F112" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="G112" t="s">
-        <v>103</v>
+        <v>306</v>
       </c>
       <c r="H112" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -3208,7 +3160,7 @@
         <v>102</v>
       </c>
       <c r="H113" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -3234,7 +3186,7 @@
         <v>102</v>
       </c>
       <c r="H114" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -3260,7 +3212,7 @@
         <v>102</v>
       </c>
       <c r="H115" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -3280,13 +3232,13 @@
         <v>1717</v>
       </c>
       <c r="F116" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="G116" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="H116" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -3306,13 +3258,13 @@
         <v>1244</v>
       </c>
       <c r="F117" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="G117" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="H117" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -3332,13 +3284,13 @@
         <v>1165</v>
       </c>
       <c r="F118" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="G118" t="s">
-        <v>102</v>
+        <v>305</v>
       </c>
       <c r="H118" t="s">
-        <v>126</v>
+        <v>163</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -3364,7 +3316,7 @@
         <v>102</v>
       </c>
       <c r="H119" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -3390,67 +3342,67 @@
         <v>102</v>
       </c>
       <c r="H120" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>12</v>
       </c>
-      <c r="B121" s="5" t="s">
-        <v>188</v>
+      <c r="B121" s="4" t="s">
+        <v>161</v>
       </c>
       <c r="C121" t="s">
         <v>100</v>
       </c>
       <c r="D121" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E121" s="2">
         <v>7746</v>
       </c>
       <c r="H121" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>13</v>
       </c>
-      <c r="B122" s="5" t="s">
-        <v>189</v>
+      <c r="B122" s="4" t="s">
+        <v>165</v>
       </c>
       <c r="C122" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="D122" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E122" s="2">
-        <v>7315</v>
+        <v>6873</v>
       </c>
       <c r="H122" t="s">
-        <v>128</v>
+        <v>163</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>14</v>
       </c>
-      <c r="B123" s="3" t="s">
-        <v>192</v>
+      <c r="B123" s="4" t="s">
+        <v>166</v>
       </c>
       <c r="C123" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="D123" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E123" s="2">
-        <v>6873</v>
+        <v>7718</v>
       </c>
       <c r="H123" t="s">
-        <v>190</v>
+        <v>167</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -3458,19 +3410,19 @@
         <v>15</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C124" t="s">
-        <v>149</v>
+        <v>164</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="D124" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E124" s="2">
         <v>7806</v>
       </c>
       <c r="H124" t="s">
-        <v>190</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3478,402 +3430,390 @@
         <v>16</v>
       </c>
       <c r="B125" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="C125" t="s">
-        <v>135</v>
+        <v>324</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="D125" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E125" s="2">
-        <v>7718</v>
+        <v>7356</v>
       </c>
       <c r="H125" t="s">
-        <v>194</v>
+        <v>116</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>17</v>
       </c>
-      <c r="B126" t="s">
-        <v>150</v>
-      </c>
-      <c r="C126" t="s">
+      <c r="B126" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C126" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D126" t="s">
-        <v>226</v>
+      <c r="D126" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E126" s="2">
         <v>7573</v>
       </c>
       <c r="H126" t="s">
-        <v>195</v>
+        <v>116</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>18</v>
       </c>
-      <c r="B127" t="s">
-        <v>241</v>
-      </c>
-      <c r="C127" t="s">
-        <v>239</v>
-      </c>
-      <c r="D127" t="s">
-        <v>230</v>
+      <c r="B127" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D127" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E127" s="2">
-        <v>7491</v>
+        <v>7315</v>
       </c>
       <c r="H127" t="s">
-        <v>322</v>
+        <v>115</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B128" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="C128" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="D128" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E128" s="2">
+        <v>7491</v>
+      </c>
+      <c r="H128" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>21</v>
+      </c>
+      <c r="B129" t="s">
+        <v>198</v>
+      </c>
+      <c r="C129" t="s">
+        <v>196</v>
+      </c>
+      <c r="D129" t="s">
+        <v>188</v>
+      </c>
+      <c r="E129" s="2">
         <v>8126</v>
       </c>
-      <c r="H128" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>224</v>
-      </c>
-      <c r="B130" t="s">
-        <v>225</v>
+      <c r="H129" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>342</v>
+        <v>185</v>
       </c>
       <c r="B131" t="s">
-        <v>344</v>
+        <v>186</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>343</v>
-      </c>
-      <c r="B132" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B137" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B138" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>223</v>
-      </c>
-      <c r="B138" t="s">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>184</v>
+      </c>
+      <c r="B139" t="s">
         <v>1</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C139" t="s">
         <v>2</v>
       </c>
-      <c r="D138" t="s">
+      <c r="D139" t="s">
         <v>3</v>
       </c>
-      <c r="E138" t="s">
+      <c r="E139" t="s">
         <v>8</v>
       </c>
-      <c r="F138" t="s">
+      <c r="F139" t="s">
         <v>87</v>
       </c>
-      <c r="G138" t="s">
+      <c r="G139" t="s">
         <v>88</v>
       </c>
-      <c r="H138" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139">
-        <v>1</v>
-      </c>
-      <c r="B139" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C139" t="s">
-        <v>48</v>
-      </c>
-      <c r="D139" t="s">
-        <v>6</v>
-      </c>
-      <c r="E139" s="1">
-        <v>6378</v>
-      </c>
-      <c r="F139" t="s">
-        <v>104</v>
-      </c>
-      <c r="G139" t="s">
-        <v>107</v>
-      </c>
       <c r="H139" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A140">
-        <v>2</v>
-      </c>
-      <c r="B140" t="s">
-        <v>49</v>
+        <v>1</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C140" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D140" t="s">
         <v>6</v>
       </c>
-      <c r="E140">
-        <v>3232</v>
+      <c r="E140" s="1">
+        <v>6378</v>
       </c>
       <c r="F140" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G140" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H140" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A141">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B141" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C141" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D141" t="s">
         <v>6</v>
       </c>
       <c r="E141">
-        <v>1043</v>
+        <v>3232</v>
       </c>
       <c r="F141" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G141" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H141" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A142">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B142" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C142" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D142" t="s">
         <v>6</v>
       </c>
       <c r="E142">
-        <v>2171</v>
+        <v>1043</v>
       </c>
       <c r="F142" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G142" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H142" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A143">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B143" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C143" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D143" t="s">
         <v>6</v>
       </c>
       <c r="E143">
-        <v>2611</v>
+        <v>2171</v>
       </c>
       <c r="F143" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="G143" t="s">
-        <v>110</v>
+        <v>307</v>
       </c>
       <c r="H143" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A144">
-        <v>6</v>
-      </c>
-      <c r="B144" s="5" t="s">
-        <v>57</v>
+        <v>5</v>
+      </c>
+      <c r="B144" t="s">
+        <v>55</v>
       </c>
       <c r="C144" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="D144" t="s">
         <v>6</v>
       </c>
-      <c r="E144" s="1">
-        <v>7432</v>
+      <c r="E144">
+        <v>2611</v>
       </c>
       <c r="F144" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="G144" t="s">
-        <v>107</v>
+        <v>308</v>
       </c>
       <c r="H144" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145">
-        <v>7</v>
-      </c>
-      <c r="B145" t="s">
-        <v>58</v>
+        <v>6</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="C145" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="D145" t="s">
         <v>6</v>
       </c>
-      <c r="E145">
-        <v>2012</v>
+      <c r="E145" s="1">
+        <v>7432</v>
       </c>
       <c r="F145" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G145" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H145" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B146" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C146" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D146" t="s">
         <v>6</v>
       </c>
       <c r="E146">
-        <v>1694</v>
+        <v>2012</v>
       </c>
       <c r="F146" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G146" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H146" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B147" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C147" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="D147" t="s">
         <v>6</v>
       </c>
       <c r="E147">
-        <v>1200</v>
+        <v>1694</v>
       </c>
       <c r="F147" t="s">
+        <v>103</v>
+      </c>
+      <c r="G147" t="s">
         <v>105</v>
       </c>
-      <c r="G147" t="s">
-        <v>109</v>
-      </c>
       <c r="H147" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B148" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C148" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D148" t="s">
         <v>6</v>
       </c>
       <c r="E148">
-        <v>2961</v>
+        <v>1200</v>
       </c>
       <c r="F148" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G148" t="s">
-        <v>109</v>
+        <v>308</v>
       </c>
       <c r="H148" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A149">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B149" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C149" t="s">
         <v>54</v>
@@ -3882,24 +3822,24 @@
         <v>6</v>
       </c>
       <c r="E149">
-        <v>1884</v>
+        <v>2961</v>
       </c>
       <c r="F149" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G149" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
       <c r="H149" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A150">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B150" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C150" t="s">
         <v>54</v>
@@ -3908,24 +3848,24 @@
         <v>6</v>
       </c>
       <c r="E150">
-        <v>1266</v>
+        <v>1884</v>
       </c>
       <c r="F150" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G150" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
       <c r="H150" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B151" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C151" t="s">
         <v>54</v>
@@ -3934,24 +3874,24 @@
         <v>6</v>
       </c>
       <c r="E151">
-        <v>1146</v>
+        <v>1266</v>
       </c>
       <c r="F151" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G151" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
       <c r="H151" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A152">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B152" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C152" t="s">
         <v>54</v>
@@ -3960,536 +3900,530 @@
         <v>6</v>
       </c>
       <c r="E152">
-        <v>1014</v>
+        <v>1146</v>
       </c>
       <c r="F152" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="G152" t="s">
-        <v>109</v>
+        <v>309</v>
       </c>
       <c r="H152" t="s">
-        <v>128</v>
+        <v>167</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A153">
-        <v>15</v>
-      </c>
-      <c r="B153" s="5" t="s">
-        <v>196</v>
+        <v>14</v>
+      </c>
+      <c r="B153" t="s">
+        <v>67</v>
       </c>
       <c r="C153" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="D153" t="s">
-        <v>226</v>
-      </c>
-      <c r="E153" s="2">
-        <v>7494</v>
+        <v>6</v>
+      </c>
+      <c r="E153">
+        <v>1014</v>
+      </c>
+      <c r="F153" t="s">
+        <v>121</v>
+      </c>
+      <c r="G153" t="s">
+        <v>310</v>
       </c>
       <c r="H153" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A154">
-        <v>16</v>
-      </c>
-      <c r="B154" s="5" t="s">
-        <v>197</v>
+        <v>15</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>168</v>
       </c>
       <c r="C154" t="s">
-        <v>146</v>
+        <v>103</v>
       </c>
       <c r="D154" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E154" s="2">
-        <v>7419</v>
+        <v>7494</v>
       </c>
       <c r="H154" t="s">
-        <v>194</v>
+        <v>113</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A155">
-        <v>17</v>
-      </c>
-      <c r="B155" s="5" t="s">
-        <v>198</v>
+        <v>16</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="C155" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D155" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E155" s="2">
-        <v>7463</v>
+        <v>7419</v>
       </c>
       <c r="H155" t="s">
-        <v>126</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A156">
-        <v>18</v>
-      </c>
-      <c r="B156" t="s">
-        <v>200</v>
+        <v>17</v>
+      </c>
+      <c r="B156" s="5" t="s">
+        <v>172</v>
       </c>
       <c r="C156" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="D156" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E156" s="2">
         <v>7438</v>
       </c>
       <c r="H156" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A157">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B157" s="5" t="s">
-        <v>148</v>
+        <v>311</v>
       </c>
       <c r="C157" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="D157" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E157" s="2">
-        <v>7394</v>
+        <v>7153</v>
       </c>
       <c r="H157" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A158">
-        <v>20</v>
-      </c>
-      <c r="B158" t="s">
-        <v>201</v>
+        <v>19</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="C158" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="D158" t="s">
-        <v>226</v>
-      </c>
-      <c r="E158">
-        <v>1770</v>
+        <v>187</v>
+      </c>
+      <c r="E158" s="2">
+        <v>7422</v>
       </c>
       <c r="H158" t="s">
-        <v>128</v>
+        <v>171</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A159">
-        <v>21</v>
-      </c>
-      <c r="B159" t="s">
-        <v>202</v>
+        <v>20</v>
+      </c>
+      <c r="B159" s="5" t="s">
+        <v>320</v>
       </c>
       <c r="C159" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D159" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E159" s="2">
-        <v>6865</v>
+        <v>6175</v>
       </c>
       <c r="H159" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A160">
-        <v>22</v>
-      </c>
-      <c r="B160" t="s">
-        <v>147</v>
+        <v>21</v>
+      </c>
+      <c r="B160" s="5" t="s">
+        <v>170</v>
       </c>
       <c r="C160" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D160" t="s">
-        <v>226</v>
-      </c>
-      <c r="E160">
-        <v>2729</v>
+        <v>187</v>
+      </c>
+      <c r="E160" s="2">
+        <v>7463</v>
       </c>
       <c r="H160" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A161">
+        <v>22</v>
+      </c>
+      <c r="B161" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C161" t="s">
+        <v>104</v>
+      </c>
+      <c r="D161" t="s">
+        <v>187</v>
+      </c>
+      <c r="E161" s="2">
+        <v>6865</v>
+      </c>
+      <c r="H161" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162">
         <v>23</v>
       </c>
-      <c r="B161" t="s">
-        <v>237</v>
-      </c>
-      <c r="C161" t="s">
-        <v>238</v>
-      </c>
-      <c r="D161" t="s">
-        <v>230</v>
-      </c>
-      <c r="E161" s="2">
+      <c r="B162" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C162" t="s">
+        <v>322</v>
+      </c>
+      <c r="D162" t="s">
+        <v>187</v>
+      </c>
+      <c r="E162" s="2">
+        <v>7212</v>
+      </c>
+      <c r="H162" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>24</v>
+      </c>
+      <c r="B163" t="s">
+        <v>193</v>
+      </c>
+      <c r="C163" t="s">
+        <v>194</v>
+      </c>
+      <c r="D163" t="s">
+        <v>188</v>
+      </c>
+      <c r="E163" s="2">
         <v>7433</v>
       </c>
-      <c r="H161" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E162" s="3"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>224</v>
-      </c>
-      <c r="B163" t="s">
-        <v>225</v>
+      <c r="H163" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A164" t="s">
-        <v>345</v>
-      </c>
-      <c r="B164" t="s">
-        <v>347</v>
-      </c>
+      <c r="E164" s="5"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>346</v>
+        <v>185</v>
       </c>
       <c r="B165" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B169" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B171" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A170" t="s">
-        <v>223</v>
-      </c>
-      <c r="B170" t="s">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>184</v>
+      </c>
+      <c r="B172" t="s">
         <v>1</v>
       </c>
-      <c r="C170" t="s">
+      <c r="C172" t="s">
         <v>2</v>
       </c>
-      <c r="D170" t="s">
+      <c r="D172" t="s">
         <v>3</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E172" t="s">
         <v>8</v>
       </c>
-      <c r="F170" t="s">
+      <c r="F172" t="s">
         <v>87</v>
       </c>
-      <c r="G170" t="s">
+      <c r="G172" t="s">
         <v>88</v>
       </c>
-      <c r="H170" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A171">
+      <c r="H172" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A173">
         <v>1</v>
       </c>
-      <c r="B171" s="5" t="s">
+      <c r="B173" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C171" t="s">
+      <c r="C173" t="s">
         <v>70</v>
       </c>
-      <c r="D171" t="s">
-        <v>6</v>
-      </c>
-      <c r="E171" s="1">
+      <c r="D173" t="s">
+        <v>6</v>
+      </c>
+      <c r="E173" s="1">
         <v>7085</v>
       </c>
-      <c r="F171" t="s">
-        <v>111</v>
-      </c>
-      <c r="G171" t="s">
-        <v>112</v>
-      </c>
-      <c r="H171" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A172">
+      <c r="F173" t="s">
+        <v>118</v>
+      </c>
+      <c r="G173" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H173" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A174">
         <v>2</v>
       </c>
-      <c r="B172" s="5" t="s">
+      <c r="B174" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C172" t="s">
+      <c r="C174" t="s">
         <v>72</v>
       </c>
-      <c r="D172" t="s">
-        <v>6</v>
-      </c>
-      <c r="E172" s="1">
+      <c r="D174" t="s">
+        <v>6</v>
+      </c>
+      <c r="E174" s="1">
         <v>7294</v>
       </c>
-      <c r="F172" t="s">
-        <v>111</v>
-      </c>
-      <c r="G172" t="s">
-        <v>113</v>
-      </c>
-      <c r="H172" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A173">
+      <c r="F174" t="s">
+        <v>118</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="H174" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" ht="17" x14ac:dyDescent="0.2">
+      <c r="A175">
         <v>3</v>
       </c>
-      <c r="B173" s="5" t="s">
+      <c r="B175" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C175" t="s">
         <v>74</v>
       </c>
-      <c r="D173" t="s">
-        <v>6</v>
-      </c>
-      <c r="E173" s="1">
+      <c r="D175" t="s">
+        <v>6</v>
+      </c>
+      <c r="E175" s="1">
         <v>7228</v>
       </c>
-      <c r="F173" t="s">
-        <v>111</v>
-      </c>
-      <c r="G173" t="s">
-        <v>112</v>
-      </c>
-      <c r="H173" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A174">
-        <v>4</v>
-      </c>
-      <c r="B174" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="C174" t="s">
-        <v>111</v>
-      </c>
-      <c r="D174" t="s">
-        <v>226</v>
-      </c>
-      <c r="E174" s="2">
-        <v>6632</v>
-      </c>
-      <c r="H174" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A175">
-        <v>5</v>
-      </c>
-      <c r="B175" s="5" t="s">
-        <v>203</v>
-      </c>
-      <c r="C175" t="s">
-        <v>111</v>
-      </c>
-      <c r="D175" t="s">
-        <v>226</v>
-      </c>
-      <c r="E175" s="2">
-        <v>6626</v>
+      <c r="F175" t="s">
+        <v>118</v>
+      </c>
+      <c r="G175" s="6" t="s">
+        <v>314</v>
       </c>
       <c r="H175" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A176">
-        <v>6</v>
-      </c>
-      <c r="B176" s="5" t="s">
-        <v>204</v>
+        <v>4</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="C176" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="D176" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E176" s="2">
-        <v>6891</v>
+        <v>6632</v>
       </c>
       <c r="H176" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A177">
+        <v>5</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C177" t="s">
+        <v>118</v>
+      </c>
+      <c r="D177" t="s">
+        <v>187</v>
+      </c>
+      <c r="E177" s="2">
+        <v>6954</v>
+      </c>
+      <c r="H177" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>6</v>
+      </c>
+      <c r="B178" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E178" s="1">
+        <v>6684</v>
+      </c>
+      <c r="H178" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A179">
         <v>7</v>
       </c>
-      <c r="B177" t="s">
-        <v>206</v>
-      </c>
-      <c r="C177" t="s">
-        <v>111</v>
-      </c>
-      <c r="D177" t="s">
-        <v>226</v>
-      </c>
-      <c r="E177" s="2">
-        <v>6684</v>
-      </c>
-      <c r="H177" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A178">
+      <c r="B179" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E179" s="1">
+        <v>6626</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A180">
         <v>8</v>
       </c>
-      <c r="B178" t="s">
-        <v>207</v>
-      </c>
-      <c r="C178" t="s">
-        <v>138</v>
-      </c>
-      <c r="D178" t="s">
-        <v>226</v>
-      </c>
-      <c r="E178" s="2">
-        <v>6766</v>
-      </c>
-      <c r="H178" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A179">
-        <v>9</v>
-      </c>
-      <c r="B179" t="s">
-        <v>142</v>
-      </c>
-      <c r="C179" t="s">
-        <v>111</v>
-      </c>
-      <c r="D179" t="s">
-        <v>226</v>
-      </c>
-      <c r="E179" s="2">
-        <v>6653</v>
-      </c>
-      <c r="H179" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A180">
-        <v>10</v>
-      </c>
-      <c r="B180" t="s">
-        <v>144</v>
-      </c>
-      <c r="C180" t="s">
-        <v>143</v>
-      </c>
-      <c r="D180" t="s">
-        <v>226</v>
-      </c>
-      <c r="E180">
-        <v>3167</v>
-      </c>
-      <c r="H180" t="s">
-        <v>209</v>
+      <c r="B180" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C180" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D180" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E180" s="1">
+        <v>6891</v>
+      </c>
+      <c r="H180" s="5" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A181">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B181" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
       <c r="C181" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
       <c r="D181" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E181" s="2">
         <v>6931</v>
       </c>
       <c r="H181" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A182">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B182" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
       <c r="C182" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
       <c r="D182" t="s">
-        <v>230</v>
+        <v>188</v>
       </c>
       <c r="E182" s="2">
         <v>7154</v>
       </c>
       <c r="H182" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
       <c r="B184" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>348</v>
-      </c>
-      <c r="B185" t="s">
-        <v>350</v>
+        <v>301</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>349</v>
-      </c>
-      <c r="B186" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -4499,7 +4433,7 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
       <c r="B191" t="s">
         <v>1</v>
@@ -4520,14 +4454,14 @@
         <v>88</v>
       </c>
       <c r="H191" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>1</v>
       </c>
-      <c r="B192" s="5" t="s">
+      <c r="B192" s="4" t="s">
         <v>76</v>
       </c>
       <c r="C192" t="s">
@@ -4540,20 +4474,20 @@
         <v>7280</v>
       </c>
       <c r="F192" t="s">
-        <v>114</v>
-      </c>
-      <c r="G192" t="s">
-        <v>117</v>
-      </c>
-      <c r="H192" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G192" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H192" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>2</v>
       </c>
-      <c r="B193" s="5" t="s">
+      <c r="B193" s="4" t="s">
         <v>78</v>
       </c>
       <c r="C193" t="s">
@@ -4566,16 +4500,16 @@
         <v>7614</v>
       </c>
       <c r="F193" t="s">
-        <v>114</v>
-      </c>
-      <c r="G193" t="s">
-        <v>117</v>
-      </c>
-      <c r="H193" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G193" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H193" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>3</v>
       </c>
@@ -4592,20 +4526,20 @@
         <v>1028</v>
       </c>
       <c r="F194" t="s">
-        <v>116</v>
-      </c>
-      <c r="G194" t="s">
         <v>118</v>
       </c>
-      <c r="H194" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G194" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="H194" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="195" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>4</v>
       </c>
-      <c r="B195" s="5" t="s">
+      <c r="B195" s="4" t="s">
         <v>81</v>
       </c>
       <c r="C195" t="s">
@@ -4618,16 +4552,16 @@
         <v>7513</v>
       </c>
       <c r="F195" t="s">
-        <v>114</v>
-      </c>
-      <c r="G195" t="s">
-        <v>117</v>
-      </c>
-      <c r="H195" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G195" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H195" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="196" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>5</v>
       </c>
@@ -4644,16 +4578,16 @@
         <v>2410</v>
       </c>
       <c r="F196" t="s">
-        <v>115</v>
-      </c>
-      <c r="G196" t="s">
-        <v>119</v>
-      </c>
-      <c r="H196" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G196" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="H196" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="197" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>6</v>
       </c>
@@ -4670,16 +4604,16 @@
         <v>2384</v>
       </c>
       <c r="F197" t="s">
-        <v>115</v>
-      </c>
-      <c r="G197" t="s">
-        <v>120</v>
-      </c>
-      <c r="H197" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G197" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H197" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="198" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>7</v>
       </c>
@@ -4696,297 +4630,214 @@
         <v>1160</v>
       </c>
       <c r="F198" t="s">
-        <v>115</v>
-      </c>
-      <c r="G198" t="s">
-        <v>121</v>
-      </c>
-      <c r="H198" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="G198" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="H198" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>8</v>
       </c>
-      <c r="B199" s="5" t="s">
-        <v>210</v>
+      <c r="B199" s="4" t="s">
+        <v>319</v>
       </c>
       <c r="C199" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="D199" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E199" s="2">
-        <v>7791</v>
-      </c>
-      <c r="H199" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7670</v>
+      </c>
+      <c r="H199" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>9</v>
       </c>
-      <c r="B200" s="5" t="s">
-        <v>213</v>
+      <c r="B200" s="4" t="s">
+        <v>178</v>
       </c>
       <c r="C200" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="D200" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E200" s="2">
-        <v>7748</v>
-      </c>
-      <c r="H200" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7791</v>
+      </c>
+      <c r="H200" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>10</v>
       </c>
       <c r="B201" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="C201" t="s">
-        <v>115</v>
-      </c>
-      <c r="D201" t="s">
-        <v>226</v>
+        <v>326</v>
+      </c>
+      <c r="C201" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D201" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E201" s="2">
-        <v>7749</v>
-      </c>
-      <c r="H201" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7611</v>
+      </c>
+      <c r="H201" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="202" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>11</v>
       </c>
-      <c r="B202" t="s">
-        <v>215</v>
-      </c>
-      <c r="C202" t="s">
-        <v>137</v>
-      </c>
-      <c r="D202" t="s">
-        <v>226</v>
+      <c r="B202" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="C202" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D202" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E202" s="2">
-        <v>7829</v>
-      </c>
-      <c r="H202" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7693</v>
+      </c>
+      <c r="H202" s="5" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="203" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>12</v>
       </c>
       <c r="B203" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="C203" t="s">
-        <v>114</v>
-      </c>
-      <c r="D203" t="s">
-        <v>226</v>
+        <v>328</v>
+      </c>
+      <c r="C203" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D203" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E203" s="2">
-        <v>7750</v>
-      </c>
-      <c r="H203" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+        <v>6945</v>
+      </c>
+      <c r="H203" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="204" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>13</v>
       </c>
-      <c r="B204" t="s">
-        <v>216</v>
+      <c r="B204" s="5" t="s">
+        <v>181</v>
       </c>
       <c r="C204" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D204" t="s">
-        <v>226</v>
+        <v>187</v>
       </c>
       <c r="E204" s="2">
-        <v>7970</v>
-      </c>
+        <v>7748</v>
+      </c>
+      <c r="F204"/>
+      <c r="G204"/>
       <c r="H204" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+      <c r="I204"/>
+    </row>
+    <row r="205" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>14</v>
       </c>
-      <c r="B205" t="s">
-        <v>217</v>
-      </c>
-      <c r="C205" t="s">
-        <v>115</v>
-      </c>
-      <c r="D205" t="s">
-        <v>226</v>
+      <c r="B205" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="C205" s="5" t="s">
+        <v>329</v>
+      </c>
+      <c r="D205" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E205" s="2">
-        <v>7672</v>
-      </c>
-      <c r="H205" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7107</v>
+      </c>
+      <c r="H205" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="206" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>15</v>
       </c>
-      <c r="B206" t="s">
-        <v>218</v>
-      </c>
-      <c r="C206" t="s">
-        <v>115</v>
-      </c>
-      <c r="D206" t="s">
-        <v>226</v>
+      <c r="B206" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="C206" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D206" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E206" s="2">
-        <v>7853</v>
-      </c>
-      <c r="H206" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+        <v>7719</v>
+      </c>
+      <c r="H206" s="5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="207" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>16</v>
       </c>
-      <c r="B207" t="s">
-        <v>139</v>
-      </c>
-      <c r="C207" t="s">
-        <v>137</v>
-      </c>
-      <c r="D207" t="s">
-        <v>226</v>
+      <c r="B207" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="C207" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D207" s="5" t="s">
+        <v>187</v>
       </c>
       <c r="E207" s="2">
-        <v>7345</v>
-      </c>
-      <c r="H207" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A208">
-        <v>17</v>
-      </c>
-      <c r="B208" t="s">
-        <v>141</v>
-      </c>
-      <c r="C208" t="s">
-        <v>140</v>
-      </c>
-      <c r="D208" t="s">
-        <v>226</v>
-      </c>
-      <c r="E208" s="2">
-        <v>7743</v>
-      </c>
-      <c r="H208" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A209">
-        <v>18</v>
+        <v>7068</v>
+      </c>
+      <c r="H207" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>185</v>
       </c>
       <c r="B209" t="s">
-        <v>227</v>
-      </c>
-      <c r="C209" t="s">
-        <v>231</v>
-      </c>
-      <c r="D209" t="s">
-        <v>230</v>
-      </c>
-      <c r="E209" s="2">
-        <v>7753</v>
-      </c>
-      <c r="H209" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A210">
-        <v>19</v>
-      </c>
-      <c r="B210" t="s">
-        <v>228</v>
-      </c>
-      <c r="C210" t="s">
-        <v>232</v>
-      </c>
-      <c r="D210" t="s">
-        <v>230</v>
-      </c>
-      <c r="E210" s="2">
-        <v>7693</v>
-      </c>
-      <c r="H210" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A211">
-        <v>20</v>
-      </c>
-      <c r="B211" t="s">
-        <v>229</v>
-      </c>
-      <c r="C211" t="s">
-        <v>115</v>
-      </c>
-      <c r="D211" t="s">
-        <v>230</v>
-      </c>
-      <c r="E211" s="2">
-        <v>7749</v>
-      </c>
-      <c r="H211" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A213" t="s">
-        <v>224</v>
-      </c>
-      <c r="B213" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A214" t="s">
-        <v>351</v>
-      </c>
-      <c r="B214" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A215" t="s">
-        <v>352</v>
-      </c>
-      <c r="B215" t="s">
-        <v>353</v>
+        <v>186</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>